<commit_message>
Added OS X benchmarks to graphs
</commit_message>
<xml_diff>
--- a/benchmark/results.xlsx
+++ b/benchmark/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Compiler</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>msvc19-ltcg</t>
+  </si>
+  <si>
+    <t>xcode82</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Cost of returning error up ten stack frames</a:t>
+              <a:t>Cost of returning error up ten stack frames on x64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -152,9 +155,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>gcc62-noexcept</c:v>
                 </c:pt>
@@ -175,16 +178,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>82.695040000000006</c:v>
                 </c:pt>
@@ -205,6 +211,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>92.626548</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86.842960000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -231,9 +240,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>gcc62-noexcept</c:v>
                 </c:pt>
@@ -254,16 +263,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>87.336759999999998</c:v>
                 </c:pt>
@@ -284,6 +296,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>97.907359999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93.196520000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -310,9 +325,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>gcc62-noexcept</c:v>
                 </c:pt>
@@ -333,16 +348,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>91.748040000000003</c:v>
                 </c:pt>
@@ -363,29 +381,32 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>98.821976000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.521439999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="146004992"/>
-        <c:axId val="158438144"/>
+        <c:axId val="165582336"/>
+        <c:axId val="165583872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146004992"/>
+        <c:axId val="165582336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158438144"/>
+        <c:crossAx val="165583872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158438144"/>
+        <c:axId val="165583872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -411,7 +432,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146004992"/>
+        <c:crossAx val="165582336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -434,7 +455,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -455,7 +476,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Cost of returning error up ten stack frames</a:t>
+              <a:t>Cost of returning error up ten stack frames on x64</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -488,9 +509,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>gcc62-noexcept</c:v>
                 </c:pt>
@@ -511,16 +532,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>82.695040000000006</c:v>
                 </c:pt>
@@ -541,6 +565,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>92.626548</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>86.842960000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -567,9 +594,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>gcc62-noexcept</c:v>
                 </c:pt>
@@ -590,16 +617,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>87.336759999999998</c:v>
                 </c:pt>
@@ -620,6 +650,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>97.907359999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>93.196520000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,9 +679,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>gcc62-noexcept</c:v>
                 </c:pt>
@@ -669,16 +702,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$9</c:f>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>91.748040000000003</c:v>
                 </c:pt>
@@ -699,6 +735,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>98.821976000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>96.521439999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,12 +762,44 @@
               <a:srgbClr val="FFFF00"/>
             </a:solidFill>
           </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>gcc62-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>gcc62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>gcc62-lto</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>clang40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>msvc19-noexcept</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>msvc19</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>msvc19-ltcg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>xcode82</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
                   <c:v>36144.941959999996</c:v>
                 </c:pt>
@@ -743,29 +814,32 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>17725.380777999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21292.326799999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="169426304"/>
-        <c:axId val="169432192"/>
+        <c:axId val="155304704"/>
+        <c:axId val="155306240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169426304"/>
+        <c:axId val="155304704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169432192"/>
+        <c:crossAx val="155306240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169432192"/>
+        <c:axId val="155306240"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -792,7 +866,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169426304"/>
+        <c:crossAx val="155304704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -815,7 +889,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1171,10 +1245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1364,6 +1438,29 @@
       </c>
       <c r="G9">
         <v>1288.5401380000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>86.842960000000005</v>
+      </c>
+      <c r="C11">
+        <v>21292.326799999999</v>
+      </c>
+      <c r="D11">
+        <v>93.196520000000007</v>
+      </c>
+      <c r="E11">
+        <v>96.521439999999998</v>
+      </c>
+      <c r="F11">
+        <v>93.920760000000001</v>
+      </c>
+      <c r="G11">
+        <v>3139.0207599999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redid benchmarks for mocked up Outcome v2 result<T>
</commit_message>
<xml_diff>
--- a/benchmark/results.xlsx
+++ b/benchmark/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="19">
   <si>
     <t>Compiler</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>xcode82</t>
+  </si>
+  <si>
+    <t>result-error-value</t>
+  </si>
+  <si>
+    <t>result-error-error</t>
+  </si>
+  <si>
+    <t>result-excpt-value</t>
+  </si>
+  <si>
+    <t>result-excpt-error</t>
   </si>
 </sst>
 </file>
@@ -223,15 +235,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>expected-error-value</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>v1 valued error_code</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -305,18 +309,47 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+            <c:v>v2 valued error_code</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>expected-error-error</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>90.95796</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.941720000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.936999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.703159999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.305593000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.356031999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.694727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>v1 errored error_code</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -389,24 +422,61 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="165582336"/>
-        <c:axId val="165583872"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>v2 errored error_code</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>87.534279999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.110600000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.529560000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.308120000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.782396000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>101.57667499999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.379529000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="172061440"/>
+        <c:axId val="172062976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165582336"/>
+        <c:axId val="172061440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165583872"/>
+        <c:crossAx val="172062976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165583872"/>
+        <c:axId val="172062976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -432,7 +502,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165582336"/>
+        <c:crossAx val="172061440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -455,7 +525,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -577,15 +647,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>expected-error-value</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>v1 valued error_code</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -659,18 +721,47 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
+            <c:v>v2 valued error_code</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>expected-error-error</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>90.95796</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>86.941720000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.936999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.703159999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>89.305593000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>93.356031999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.694727</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>v1 errored error_code</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -744,8 +835,45 @@
           </c:val>
         </c:ser>
         <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>v2 errored error_code</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>87.534279999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.110600000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.529560000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.308120000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94.782396000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>101.57667499999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94.379529000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="3"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$C$1</c:f>
@@ -822,24 +950,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="155304704"/>
-        <c:axId val="155306240"/>
+        <c:axId val="172319872"/>
+        <c:axId val="172321408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="155304704"/>
+        <c:axId val="172319872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155306240"/>
+        <c:crossAx val="172321408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="155306240"/>
+        <c:axId val="172321408"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -866,7 +994,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="155304704"/>
+        <c:crossAx val="172319872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -889,7 +1017,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1245,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1262,7 +1390,7 @@
     <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1284,8 +1412,20 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1304,8 +1444,20 @@
       <c r="G2">
         <v>105.44276000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>90.95796</v>
+      </c>
+      <c r="I2">
+        <v>87.534279999999995</v>
+      </c>
+      <c r="J2">
+        <v>100.37308</v>
+      </c>
+      <c r="K2">
+        <v>93.986599999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1327,8 +1479,20 @@
       <c r="G3">
         <v>5233.5886799999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>86.941720000000004</v>
+      </c>
+      <c r="I3">
+        <v>84.110600000000005</v>
+      </c>
+      <c r="J3">
+        <v>89.213200000000001</v>
+      </c>
+      <c r="K3">
+        <v>3743.9257600000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1350,8 +1514,20 @@
       <c r="G4">
         <v>4891.1219199999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>97.936999999999998</v>
+      </c>
+      <c r="I4">
+        <v>98.529560000000004</v>
+      </c>
+      <c r="J4">
+        <v>93.525720000000007</v>
+      </c>
+      <c r="K4">
+        <v>3755.7769600000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1373,8 +1549,20 @@
       <c r="G5">
         <v>4665.6528399999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H5">
+        <v>84.703159999999997</v>
+      </c>
+      <c r="I5">
+        <v>84.308120000000002</v>
+      </c>
+      <c r="J5">
+        <v>103.46756000000001</v>
+      </c>
+      <c r="K5">
+        <v>293.67932000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1393,8 +1581,20 @@
       <c r="G7">
         <v>1234.403638</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>89.305593000000002</v>
+      </c>
+      <c r="I7">
+        <v>94.782396000000006</v>
+      </c>
+      <c r="J7">
+        <v>94.205316999999994</v>
+      </c>
+      <c r="K7">
+        <v>1195.5756570000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1416,8 +1616,20 @@
       <c r="G8">
         <v>1360.544294</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8">
+        <v>93.356031999999999</v>
+      </c>
+      <c r="I8">
+        <v>101.57667499999999</v>
+      </c>
+      <c r="J8">
+        <v>99.290138999999996</v>
+      </c>
+      <c r="K8">
+        <v>1246.4456580000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1439,8 +1651,20 @@
       <c r="G9">
         <v>1288.5401380000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H9">
+        <v>100.694727</v>
+      </c>
+      <c r="I9">
+        <v>94.379529000000005</v>
+      </c>
+      <c r="J9">
+        <v>90.535968999999994</v>
+      </c>
+      <c r="K9">
+        <v>1200.823805</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1471,12 +1695,512 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>90.003280000000004</v>
+      </c>
+      <c r="D2">
+        <v>93.36112</v>
+      </c>
+      <c r="E2">
+        <v>96.620199999999997</v>
+      </c>
+      <c r="F2">
+        <v>100.83396</v>
+      </c>
+      <c r="G2">
+        <v>114.03488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>87.962239999999994</v>
+      </c>
+      <c r="C3">
+        <v>32873.220679999999</v>
+      </c>
+      <c r="D3">
+        <v>85.295720000000003</v>
+      </c>
+      <c r="E3">
+        <v>90.266639999999995</v>
+      </c>
+      <c r="F3">
+        <v>85.49324</v>
+      </c>
+      <c r="G3">
+        <v>4479.0951999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>98.134519999999995</v>
+      </c>
+      <c r="C4">
+        <v>3764.2044799999999</v>
+      </c>
+      <c r="D4">
+        <v>98.430800000000005</v>
+      </c>
+      <c r="E4">
+        <v>98.364959999999996</v>
+      </c>
+      <c r="F4">
+        <v>98.101600000000005</v>
+      </c>
+      <c r="G4">
+        <v>3904.8716399999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>85.756600000000006</v>
+      </c>
+      <c r="C5">
+        <v>32076.721280000002</v>
+      </c>
+      <c r="D5">
+        <v>89.937439999999995</v>
+      </c>
+      <c r="E5">
+        <v>91.418840000000003</v>
+      </c>
+      <c r="F5">
+        <v>101.26192</v>
+      </c>
+      <c r="G5">
+        <v>292.13207999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>82.695040000000006</v>
+      </c>
+      <c r="D8">
+        <v>90.95796</v>
+      </c>
+      <c r="E8">
+        <v>87.534279999999995</v>
+      </c>
+      <c r="F8">
+        <v>100.37308</v>
+      </c>
+      <c r="G8">
+        <v>93.986599999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>83.188839999999999</v>
+      </c>
+      <c r="C9">
+        <v>32838.292560000002</v>
+      </c>
+      <c r="D9">
+        <v>86.941720000000004</v>
+      </c>
+      <c r="E9">
+        <v>84.110600000000005</v>
+      </c>
+      <c r="F9">
+        <v>89.213200000000001</v>
+      </c>
+      <c r="G9">
+        <v>3743.9257600000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>92.801479999999998</v>
+      </c>
+      <c r="C10">
+        <v>3550.4549200000001</v>
+      </c>
+      <c r="D10">
+        <v>97.936999999999998</v>
+      </c>
+      <c r="E10">
+        <v>98.529560000000004</v>
+      </c>
+      <c r="F10">
+        <v>93.525720000000007</v>
+      </c>
+      <c r="G10">
+        <v>3755.7769600000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>85.888279999999995</v>
+      </c>
+      <c r="C11">
+        <v>31827.220600000001</v>
+      </c>
+      <c r="D11">
+        <v>84.703159999999997</v>
+      </c>
+      <c r="E11">
+        <v>84.308120000000002</v>
+      </c>
+      <c r="F11">
+        <v>103.46756000000001</v>
+      </c>
+      <c r="G11">
+        <v>293.67932000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>87.628800999999996</v>
+      </c>
+      <c r="D14">
+        <v>91.330811999999995</v>
+      </c>
+      <c r="E14">
+        <v>89.262044000000003</v>
+      </c>
+      <c r="F14">
+        <v>88.597855999999993</v>
+      </c>
+      <c r="G14">
+        <v>1160.0036789999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>81.640253999999999</v>
+      </c>
+      <c r="C15">
+        <v>16670.922133</v>
+      </c>
+      <c r="D15">
+        <v>92.561188000000001</v>
+      </c>
+      <c r="E15">
+        <v>89.174937</v>
+      </c>
+      <c r="F15">
+        <v>103.645448</v>
+      </c>
+      <c r="G15">
+        <v>1216.0347180000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>94.629958999999999</v>
+      </c>
+      <c r="C16">
+        <v>16559.742001999999</v>
+      </c>
+      <c r="D16">
+        <v>94.967495999999997</v>
+      </c>
+      <c r="E16">
+        <v>92.016774999999996</v>
+      </c>
+      <c r="F16">
+        <v>90.089550000000003</v>
+      </c>
+      <c r="G16">
+        <v>1199.3321129999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>80.126783000000003</v>
+      </c>
+      <c r="D19">
+        <v>92.757176999999999</v>
+      </c>
+      <c r="E19">
+        <v>87.726795999999993</v>
+      </c>
+      <c r="F19">
+        <v>91.799008000000001</v>
+      </c>
+      <c r="G19">
+        <v>1213.3235380000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>81.847130000000007</v>
+      </c>
+      <c r="C20">
+        <v>17323.205754999999</v>
+      </c>
+      <c r="D20">
+        <v>101.206475</v>
+      </c>
+      <c r="E20">
+        <v>103.144588</v>
+      </c>
+      <c r="F20">
+        <v>136.77845400000001</v>
+      </c>
+      <c r="G20">
+        <v>1220.542461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>98.223089000000002</v>
+      </c>
+      <c r="C21">
+        <v>16924.727718999999</v>
+      </c>
+      <c r="D21">
+        <v>97.983545000000007</v>
+      </c>
+      <c r="E21">
+        <v>93.443139000000002</v>
+      </c>
+      <c r="F21">
+        <v>92.114769999999993</v>
+      </c>
+      <c r="G21">
+        <v>1219.246758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>94.096434000000002</v>
+      </c>
+      <c r="D24">
+        <v>89.305593000000002</v>
+      </c>
+      <c r="E24">
+        <v>94.782396000000006</v>
+      </c>
+      <c r="F24">
+        <v>94.205316999999994</v>
+      </c>
+      <c r="G24">
+        <v>1195.5756570000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>83.763463999999999</v>
+      </c>
+      <c r="C25">
+        <v>16639.618354999999</v>
+      </c>
+      <c r="D25">
+        <v>93.356031999999999</v>
+      </c>
+      <c r="E25">
+        <v>101.57667499999999</v>
+      </c>
+      <c r="F25">
+        <v>99.290138999999996</v>
+      </c>
+      <c r="G25">
+        <v>1246.4456580000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>100.368078</v>
+      </c>
+      <c r="C26">
+        <v>16770.963563000001</v>
+      </c>
+      <c r="D26">
+        <v>100.694727</v>
+      </c>
+      <c r="E26">
+        <v>94.379529000000005</v>
+      </c>
+      <c r="F26">
+        <v>90.535968999999994</v>
+      </c>
+      <c r="G26">
+        <v>1200.823805</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>